<commit_message>
first commit git chek-in
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\baswangudi\com.vtigerProject\Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19320" windowHeight="5970"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="6120" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:R20"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -547,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28:I28"/>
+    <sheetView topLeftCell="D1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1097,7 +1093,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView zoomScale="91" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="91" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>